<commit_message>
Add more partitions and reader threads and document the results.
</commit_message>
<xml_diff>
--- a/throughput.xlsx
+++ b/throughput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/randy/Documents/projects/hazelcast-certification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9166B8E4-C27D-5E4D-BC7B-254378171F29}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7AD8E0-F7D3-534C-989B-F5E3B7262651}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{63738722-5818-8F43-B05D-9165230C02A6}"/>
   </bookViews>
@@ -31,12 +31,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Nodes</t>
   </si>
   <si>
     <t>Throughput (Ktps)</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>with 2063 partitions and 192 reader threads</t>
+  </si>
+  <si>
+    <t>with 1031 partitions and 128 reader threads</t>
   </si>
 </sst>
 </file>
@@ -72,8 +81,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -106,7 +118,44 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Scaling</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Study: Servers vs. Throughput in K TPS</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.30614555407554783"/>
+          <c:y val="5.5958549222797929E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -178,6 +227,7 @@
             </c:spPr>
           </c:marker>
           <c:trendline>
+            <c:name>Quadratic Trendline (best fit)</c:name>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
@@ -195,8 +245,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.0921389109016621E-2"/>
-                  <c:y val="-7.7283332304626529E-2"/>
+                  <c:x val="-0.12652941936861747"/>
+                  <c:y val="-2.001534005140549E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -284,6 +334,128 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Improvements</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$7:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>153</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4261-CE42-B285-37C831022E66}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -316,6 +488,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Hazelcast</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Servers</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -378,6 +609,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>K</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> TPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -427,6 +717,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="l"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1031,16 +1352,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>730250</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1368,26 +1689,30 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>8</v>
       </c>
@@ -1395,7 +1720,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10</v>
       </c>
@@ -1403,7 +1728,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>12</v>
       </c>
@@ -1411,7 +1736,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>14</v>
       </c>
@@ -1419,12 +1744,34 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>16</v>
       </c>
       <c r="B6">
         <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>140</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>153</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>